<commit_message>
Correction screendump array4 and typing errors. Shortdesc for topics added / improved. Task identity matrix replaced with concept mathematical matrix functions. Minor textual corrections. Updated version info and revise date.
</commit_message>
<xml_diff>
--- a/practicefiles/Array4.xlsx
+++ b/practicefiles/Array4.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23318"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\office\LearnExcel-source\practicefiles\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C01E6700-185B-483F-81E3-A7EC03F9884F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="135" windowWidth="27840" windowHeight="12585"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -46,12 +52,18 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -75,11 +87,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -87,12 +100,15 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -134,7 +150,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -167,9 +183,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -202,6 +235,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -377,100 +427,102 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="5" width="7.7109375" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B1">
+      <c r="B1" s="1">
         <v>2</v>
       </c>
-      <c r="C1">
+      <c r="C1" s="1">
         <v>2</v>
       </c>
-      <c r="D1">
+      <c r="D1" s="1">
         <v>3</v>
       </c>
-      <c r="E1">
+      <c r="E1" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B2" t="s">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="1">
         <v>6</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="1">
         <v>7</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="1">
         <v>5</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="1">
         <v>7</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="1">
         <v>5</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="1">
         <v>6</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="1">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="1">
         <v>8</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="1">
         <v>8</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="1">
         <v>6</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="1">
         <v>7</v>
       </c>
     </row>

</xml_diff>